<commit_message>
NucleotideSkew: Simple update in one of the analysis files
</commit_message>
<xml_diff>
--- a/NucleotideSkew/AnalysedCodonDistributionPerStrand.xlsx
+++ b/NucleotideSkew/AnalysedCodonDistributionPerStrand.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="CodonDistribution" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t xml:space="preserve"> Format: Codon</t>
   </si>
@@ -260,6 +260,36 @@
   </si>
   <si>
     <t>End with C</t>
+  </si>
+  <si>
+    <t>Middle with A</t>
+  </si>
+  <si>
+    <t>Middle with T</t>
+  </si>
+  <si>
+    <t>Middle with G</t>
+  </si>
+  <si>
+    <t>Middle with C</t>
+  </si>
+  <si>
+    <t>Pgene+Ngene</t>
+  </si>
+  <si>
+    <t>ProteinPGene+ProteinNGene</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K78"/>
+  <dimension ref="B2:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="L72" sqref="L72"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="L88" sqref="L88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,6 +2845,14 @@
         <v>683043</v>
       </c>
     </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I69" t="s">
+        <v>86</v>
+      </c>
+      <c r="J69" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>72</v>
@@ -2847,6 +2885,10 @@
         <f>SUM(D70,H70)</f>
         <v>314143</v>
       </c>
+      <c r="J70">
+        <f>SUM(C70+F70)</f>
+        <v>303417</v>
+      </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
@@ -2877,8 +2919,12 @@
         <v>176985</v>
       </c>
       <c r="I71">
-        <f t="shared" ref="I71:I78" si="2">SUM(D71,H71)</f>
+        <f t="shared" ref="I71:I83" si="2">SUM(D71,H71)</f>
         <v>333237</v>
+      </c>
+      <c r="J71">
+        <f t="shared" ref="J71:J73" si="3">SUM(C71+F71)</f>
+        <v>280866</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
@@ -2890,29 +2936,33 @@
         <v>221304</v>
       </c>
       <c r="D72">
-        <f t="shared" ref="D72:H72" si="3">SUM(D35:D50)</f>
+        <f t="shared" ref="D72:H72" si="4">SUM(D35:D50)</f>
         <v>182813</v>
       </c>
       <c r="E72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3243</v>
       </c>
       <c r="F72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>159708</v>
       </c>
       <c r="G72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1214</v>
       </c>
       <c r="H72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>161203</v>
       </c>
       <c r="I72">
         <f t="shared" si="2"/>
         <v>344016</v>
       </c>
+      <c r="J72">
+        <f t="shared" si="3"/>
+        <v>381012</v>
+      </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
@@ -2923,160 +2973,380 @@
         <v>155021</v>
       </c>
       <c r="D73">
-        <f t="shared" ref="D73:H73" si="4">SUM(D51:D66)</f>
+        <f t="shared" ref="D73:H73" si="5">SUM(D51:D66)</f>
         <v>163683</v>
       </c>
       <c r="E73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2525</v>
       </c>
       <c r="F73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>195265</v>
       </c>
       <c r="G73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1563</v>
       </c>
       <c r="H73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>176146</v>
       </c>
       <c r="I73">
         <f t="shared" si="2"/>
         <v>339829</v>
       </c>
+      <c r="J73">
+        <f t="shared" si="3"/>
+        <v>350286</v>
+      </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75">
+        <f>SUM(C3,C4,C5,C6,C19,C20,C21,C22,C35,C36,C37,C38,C51,C52,C53,C54)</f>
+        <v>183288</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:I75" si="6">SUM(D3,D4,D5,D6,D19,D20,D21,D22,D35,D36,D37,D38,D51,D52,D53,D54)</f>
+        <v>159158</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="6"/>
+        <v>2621</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="6"/>
+        <v>193033</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="6"/>
+        <v>1123</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="6"/>
+        <v>177020</v>
+      </c>
+      <c r="I75">
+        <f>SUM(D75,H75)</f>
+        <v>336178</v>
+      </c>
+      <c r="J75">
+        <f>SUM(C75+F75)</f>
+        <v>376321</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>83</v>
+      </c>
+      <c r="C76">
+        <f>SUM(C7,C8,C9,C10,C23,C24,C25,C26,C39,C40,C41,C42,C55,C56,C57,C58)</f>
+        <v>194628</v>
+      </c>
+      <c r="D76">
+        <f t="shared" ref="D76:I76" si="7">SUM(D7,D8,D9,D10,D23,D24,D25,D26,D39,D40,D41,D42,D55,D56,D57,D58)</f>
+        <v>141856</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="7"/>
+        <v>2422</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="7"/>
+        <v>167591</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="7"/>
+        <v>1234</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="7"/>
+        <v>155178</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="2"/>
+        <v>297034</v>
+      </c>
+      <c r="J76">
+        <f t="shared" ref="J76:J78" si="8">SUM(C76+F76)</f>
+        <v>362219</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77">
+        <f>SUM(C11,C12,C13,C14,C27,C28,C29,C30,C43,C44,C45,C46,C59,C60,C61,C62)</f>
+        <v>115291</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ref="D77:I77" si="9">SUM(D11,D12,D13,D14,D27,D28,D29,D30,D43,D44,D45,D46,D59,D60,D61,D62)</f>
+        <v>187788</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="9"/>
+        <v>3221</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="9"/>
+        <v>165494</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="9"/>
+        <v>1223</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="9"/>
+        <v>172521</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="2"/>
+        <v>360309</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="8"/>
+        <v>280785</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78">
+        <f>SUM(C15,C16,C17,C18,C31,C32,C33,C34,C47,C48,C49,C50,C63,C64,C65,C66)</f>
+        <v>144373</v>
+      </c>
+      <c r="D78">
+        <f t="shared" ref="D78:I78" si="10">SUM(D15,D16,D17,D18,D31,D32,D33,D34,D47,D48,D49,D50,D63,D64,D65,D66)</f>
+        <v>159380</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="10"/>
+        <v>2465</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="10"/>
+        <v>151883</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="10"/>
+        <v>1497</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="10"/>
+        <v>178324</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="2"/>
+        <v>337704</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="8"/>
+        <v>296256</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>78</v>
       </c>
-      <c r="C75">
+      <c r="C80">
         <f>SUM(C3,C7,C11,C15,C19,C23,C27,C31,C35,C39,C43,C47,C51,C55,C59,C63)</f>
         <v>115284</v>
       </c>
-      <c r="D75">
-        <f t="shared" ref="D75:H75" si="5">SUM(D3,D7,D11,D15,D19,D23,D27,D31,D35,D39,D43,D47,D51,D55,D59,D63)</f>
+      <c r="D80">
+        <f t="shared" ref="D80:H80" si="11">SUM(D3,D7,D11,D15,D19,D23,D27,D31,D35,D39,D43,D47,D51,D55,D59,D63)</f>
         <v>162300</v>
       </c>
-      <c r="E75">
-        <f t="shared" si="5"/>
+      <c r="E80">
+        <f t="shared" si="11"/>
         <v>2639</v>
       </c>
-      <c r="F75">
-        <f t="shared" si="5"/>
+      <c r="F80">
+        <f t="shared" si="11"/>
         <v>151986</v>
       </c>
-      <c r="G75">
-        <f t="shared" si="5"/>
+      <c r="G80">
+        <f t="shared" si="11"/>
         <v>1055</v>
       </c>
-      <c r="H75">
-        <f t="shared" si="5"/>
+      <c r="H80">
+        <f t="shared" si="11"/>
         <v>145396</v>
       </c>
-      <c r="I75">
+      <c r="I80">
         <f t="shared" si="2"/>
         <v>307696</v>
       </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="J80">
+        <f>SUM(C80+F80)</f>
+        <v>267270</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
         <v>79</v>
       </c>
-      <c r="C76">
-        <f t="shared" ref="C76:H78" si="6">SUM(C4,C8,C12,C16,C20,C24,C28,C32,C36,C40,C44,C48,C52,C56,C60,C64)</f>
+      <c r="C81">
+        <f t="shared" ref="C81:H83" si="12">SUM(C4,C8,C12,C16,C20,C24,C28,C32,C36,C40,C44,C48,C52,C56,C60,C64)</f>
         <v>165036</v>
       </c>
-      <c r="D76">
-        <f t="shared" si="6"/>
+      <c r="D81">
+        <f t="shared" si="12"/>
         <v>169257</v>
       </c>
-      <c r="E76">
-        <f t="shared" si="6"/>
+      <c r="E81">
+        <f t="shared" si="12"/>
         <v>2300</v>
       </c>
-      <c r="F76">
-        <f t="shared" si="6"/>
+      <c r="F81">
+        <f t="shared" si="12"/>
         <v>140333</v>
       </c>
-      <c r="G76">
-        <f t="shared" si="6"/>
+      <c r="G81">
+        <f t="shared" si="12"/>
         <v>1231</v>
       </c>
-      <c r="H76">
-        <f t="shared" si="6"/>
+      <c r="H81">
+        <f t="shared" si="12"/>
         <v>159585</v>
       </c>
-      <c r="I76">
+      <c r="I81">
         <f t="shared" si="2"/>
         <v>328842</v>
       </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+      <c r="J81">
+        <f t="shared" ref="J81:J83" si="13">SUM(C81+F81)</f>
+        <v>305369</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
         <v>80</v>
       </c>
-      <c r="C77">
-        <f t="shared" si="6"/>
+      <c r="C82">
+        <f t="shared" si="12"/>
         <v>186247</v>
       </c>
-      <c r="D77">
-        <f t="shared" si="6"/>
+      <c r="D82">
+        <f t="shared" si="12"/>
         <v>161870</v>
       </c>
-      <c r="E77">
-        <f t="shared" si="6"/>
+      <c r="E82">
+        <f t="shared" si="12"/>
         <v>3279</v>
       </c>
-      <c r="F77">
-        <f t="shared" si="6"/>
+      <c r="F82">
+        <f t="shared" si="12"/>
         <v>174969</v>
       </c>
-      <c r="G77">
-        <f t="shared" si="6"/>
+      <c r="G82">
+        <f t="shared" si="12"/>
         <v>1229</v>
       </c>
-      <c r="H77">
-        <f t="shared" si="6"/>
+      <c r="H82">
+        <f t="shared" si="12"/>
         <v>170084</v>
       </c>
-      <c r="I77">
+      <c r="I82">
         <f t="shared" si="2"/>
         <v>331954</v>
       </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+      <c r="J82">
+        <f t="shared" si="13"/>
+        <v>361216</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>81</v>
       </c>
-      <c r="C78">
-        <f t="shared" si="6"/>
+      <c r="C83">
+        <f t="shared" si="12"/>
         <v>171013</v>
       </c>
-      <c r="D78">
-        <f t="shared" si="6"/>
+      <c r="D83">
+        <f t="shared" si="12"/>
         <v>154755</v>
       </c>
-      <c r="E78">
-        <f t="shared" si="6"/>
+      <c r="E83">
+        <f t="shared" si="12"/>
         <v>2511</v>
       </c>
-      <c r="F78">
-        <f t="shared" si="6"/>
+      <c r="F83">
+        <f t="shared" si="12"/>
         <v>210713</v>
       </c>
-      <c r="G78">
-        <f t="shared" si="6"/>
+      <c r="G83">
+        <f t="shared" si="12"/>
         <v>1562</v>
       </c>
-      <c r="H78">
-        <f t="shared" si="6"/>
+      <c r="H83">
+        <f t="shared" si="12"/>
         <v>207978</v>
       </c>
-      <c r="I78">
+      <c r="I83">
         <f t="shared" si="2"/>
         <v>362733</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="13"/>
+        <v>381726</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>88</v>
+      </c>
+      <c r="I85">
+        <f>SUM(I70+I75+I80)</f>
+        <v>958017</v>
+      </c>
+      <c r="J85">
+        <f>SUM(J70+J75+J80)</f>
+        <v>947008</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>90</v>
+      </c>
+      <c r="I86">
+        <f t="shared" ref="I86:J88" si="14">SUM(I71+I76+I81)</f>
+        <v>959113</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="14"/>
+        <v>948454</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>89</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="14"/>
+        <v>1036279</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="14"/>
+        <v>1023013</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>91</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="14"/>
+        <v>1040266</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="14"/>
+        <v>1028268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>